<commit_message>
pagina apprendista finita + pagina formatori conclusa + diario
</commit_message>
<xml_diff>
--- a/progettazione/requisitiLPI.xlsx
+++ b/progettazione/requisitiLPI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -288,6 +288,15 @@
   </si>
   <si>
     <t>Salvare il file in pdf sul server</t>
+  </si>
+  <si>
+    <t>REQ-014</t>
+  </si>
+  <si>
+    <t>Gestione dati</t>
+  </si>
+  <si>
+    <t>Prevedere l'eliminazione definitiva dei dati flag=0 e ripristino</t>
   </si>
 </sst>
 </file>
@@ -654,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E154"/>
+  <dimension ref="B1:E162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="D157" sqref="D157"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="A154" sqref="A154:XFD154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1622,7 +1631,7 @@
         <v>4</v>
       </c>
       <c r="C150" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1649,6 +1658,59 @@
       <c r="B154" s="1"/>
       <c r="C154" s="7" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="156" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B156" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B157" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="158" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B158" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C158" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B159" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C159" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B160" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C160" s="3"/>
+    </row>
+    <row r="161" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B161" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B162" s="1"/>
+      <c r="C162" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pagina datori di lavoro, creazione pdf con tcpdf + diario e commenti ai codici
</commit_message>
<xml_diff>
--- a/progettazione/requisitiLPI.xlsx
+++ b/progettazione/requisitiLPI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LPI\progettazione\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LPI\progettazione\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Ha accesso completo al sito web</t>
   </si>
   <si>
-    <t>Può creare, modificare, eliminare dati dal sito web (da riguardare)</t>
-  </si>
-  <si>
     <t>Può eliminare gli utenti normali</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>utenti normali</t>
   </si>
   <si>
-    <t>Può modificare la propria password</t>
-  </si>
-  <si>
     <t>Può rendere gli utenti normali degli amministratori e viceversa</t>
   </si>
   <si>
@@ -122,9 +116,6 @@
     <t>Ha accesso completo al sito</t>
   </si>
   <si>
-    <t>Può cambiare la propria password</t>
-  </si>
-  <si>
     <t>Deve essere operativo online</t>
   </si>
   <si>
@@ -254,9 +245,6 @@
     <t>Le informazioni per la registrazioni sono email e password</t>
   </si>
   <si>
-    <t>Questa pagina è accessibile solo agli amministratori</t>
-  </si>
-  <si>
     <t>prevedere una pagina di modifica accessibile agli amministratori in scrittura</t>
   </si>
   <si>
@@ -266,12 +254,6 @@
     <t>Pagina apprendisti</t>
   </si>
   <si>
-    <t>Prevedere un bottone di dettaglio che mostri tutti i dati ddell'apprendista con un campo osservazioni e le indicazioni del datore di lavoro e formatore</t>
-  </si>
-  <si>
-    <t>Prevedere un bottone di modifica che mostri i dati come presenti in dettaglio ma avere per datore di lavoro e formatore solo la possibilità di cambiarli</t>
-  </si>
-  <si>
     <t>Pagina datori di lavoro</t>
   </si>
   <si>
@@ -296,7 +278,25 @@
     <t>Gestione dati</t>
   </si>
   <si>
-    <t>Prevedere l'eliminazione definitiva dei dati flag=0 e ripristino</t>
+    <t>Può cambiare la password</t>
+  </si>
+  <si>
+    <t>Solo gli amministratori possono registrare account</t>
+  </si>
+  <si>
+    <t>Prevedere un bottone di dettaglio che mostri tutti i dati dell'apprendista con un campo osservazioni e le indicazioni del datore di lavoro e formatore</t>
+  </si>
+  <si>
+    <t>Prevedere un bottone di modifica che mostri i dati presenti in dettaglio solo per datore di lavoro e formatore e</t>
+  </si>
+  <si>
+    <t>Prevedere eliminazione</t>
+  </si>
+  <si>
+    <t>prevedere conferma per eliminazione degli account</t>
+  </si>
+  <si>
+    <t>Prevedere l'eliminazione definitiva dei dati eliminati e ripristino</t>
   </si>
 </sst>
 </file>
@@ -358,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -383,6 +383,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -663,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E162"/>
+  <dimension ref="B1:E163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="A154" sqref="A154:XFD154"/>
+    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F166" sqref="F166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -754,7 +755,7 @@
     <row r="13" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6"/>
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -819,37 +820,37 @@
     <row r="24" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
       <c r="C24" s="8" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="6"/>
       <c r="C25" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6"/>
       <c r="C26" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="6"/>
       <c r="C27" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="6"/>
       <c r="C28" s="7" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="6"/>
       <c r="C29" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -858,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -866,7 +867,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -902,43 +903,43 @@
     <row r="37" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="5"/>
       <c r="C37" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="6"/>
       <c r="C38" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="6"/>
       <c r="C39" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="6"/>
       <c r="C40" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="6"/>
       <c r="C41" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="6"/>
       <c r="C42" s="7" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="6"/>
       <c r="C43" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -947,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -955,7 +956,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -991,19 +992,19 @@
     <row r="51" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="5"/>
       <c r="C51" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="6"/>
       <c r="C52" s="7" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B53" s="6"/>
       <c r="C53" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="54" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1012,7 +1013,7 @@
         <v>0</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1020,7 +1021,7 @@
         <v>2</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1056,19 +1057,19 @@
     <row r="61" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B61" s="1"/>
       <c r="C61" s="9" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B62" s="5"/>
       <c r="C62" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B63" s="6"/>
       <c r="C63" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1077,7 +1078,7 @@
         <v>0</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1085,7 +1086,7 @@
         <v>2</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1110,7 +1111,7 @@
       </c>
       <c r="C69" s="3"/>
       <c r="E69" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="70" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1124,7 +1125,7 @@
     <row r="71" spans="2:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B71" s="5"/>
       <c r="C71" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1133,7 +1134,7 @@
         <v>0</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="74" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1141,7 +1142,7 @@
         <v>2</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="75" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1177,7 +1178,7 @@
     <row r="79" spans="2:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B79" s="5"/>
       <c r="C79" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="80" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1186,7 +1187,7 @@
         <v>0</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="82" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1194,7 +1195,7 @@
         <v>2</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1230,31 +1231,31 @@
     <row r="87" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B87" s="1"/>
       <c r="C87" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="88" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B88" s="5"/>
       <c r="C88" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B89" s="5"/>
       <c r="C89" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="90" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B90" s="5"/>
       <c r="C90" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B91" s="5"/>
       <c r="C91" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="92" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1263,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="94" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1271,7 +1272,7 @@
         <v>2</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="95" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1307,49 +1308,49 @@
     <row r="99" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B99" s="1"/>
       <c r="C99" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="100" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B100" s="5"/>
       <c r="C100" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="101" spans="2:3" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B101" s="5"/>
       <c r="C101" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="102" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B102" s="5"/>
       <c r="C102" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="103" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B103" s="5"/>
       <c r="C103" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="104" spans="2:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B104" s="5"/>
       <c r="C104" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="105" spans="2:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B105" s="5"/>
       <c r="C105" s="7" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="106" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B106" s="5"/>
       <c r="C106" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="107" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1358,7 +1359,7 @@
         <v>0</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="109" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1366,7 +1367,7 @@
         <v>2</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="110" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1402,314 +1403,320 @@
     <row r="114" spans="2:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B114" s="5"/>
       <c r="C114" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="115" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B115" s="5"/>
       <c r="C115" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="116" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B116" s="5"/>
-      <c r="C116" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="117" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="118" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B118" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
+      <c r="C116" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B117" s="5"/>
+      <c r="C117" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="119" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B119" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>61</v>
+        <v>0</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="120" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B120" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C120" s="3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="121" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B121" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C121" s="4">
+        <v>3</v>
+      </c>
+      <c r="C121" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="122" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B122" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C122" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="C122" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="123" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B123" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C123" s="3"/>
+    </row>
+    <row r="124" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B124" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C124" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B124" s="1"/>
-      <c r="C124" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="125" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B125" s="1"/>
       <c r="C125" s="7" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="126" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B126" s="1"/>
       <c r="C126" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="127" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B127" s="1"/>
       <c r="C127" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="128" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B128" s="1"/>
       <c r="C128" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="129" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B129" s="1"/>
       <c r="C129" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="130" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B130" s="1"/>
       <c r="C130" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="131" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B131" s="1"/>
       <c r="C131" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="132" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="133" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B133" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B132" s="1"/>
+      <c r="C132" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="134" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B134" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C134" s="7" t="s">
-        <v>69</v>
+        <v>0</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="135" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B135" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C135" s="3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C135" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="136" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B136" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C136" s="4">
+        <v>3</v>
+      </c>
+      <c r="C136" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="137" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B137" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C137" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="C137" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="138" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B138" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C138" s="3"/>
+    </row>
+    <row r="139" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B139" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="C139" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B139" s="1"/>
-      <c r="C139" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="140" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B140" s="1"/>
       <c r="C140" s="7" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="141" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B141" s="1"/>
       <c r="C141" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="142" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B142" s="1"/>
       <c r="C142" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="143" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B143" s="1"/>
       <c r="C143" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="144" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B144" s="1"/>
       <c r="C144" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="145" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B145" s="1"/>
       <c r="C145" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="146" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="147" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B147" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B146" s="1"/>
+      <c r="C146" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="148" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B148" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C148" s="7" t="s">
-        <v>83</v>
+        <v>0</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="149" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B149" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C149" s="3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C149" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="150" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B150" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C150" s="4">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C150" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B151" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C151" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="C151" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="152" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C152" s="3"/>
+    </row>
+    <row r="153" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B153" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C152" s="2" t="s">
+      <c r="C153" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B153" s="1"/>
-      <c r="C153" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="154" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B154" s="1"/>
       <c r="C154" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="155" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="156" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B156" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B155" s="1"/>
+      <c r="C155" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="157" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B157" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C157" s="7" t="s">
-        <v>89</v>
+        <v>0</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="158" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B158" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C158" s="3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C158" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="159" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B159" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C159" s="4">
         <v>3</v>
+      </c>
+      <c r="C159" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B160" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C160" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="C160" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="161" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B161" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C161" s="3"/>
+    </row>
+    <row r="162" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B162" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C161" s="2" t="s">
+      <c r="C162" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="162" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B162" s="1"/>
-      <c r="C162" s="7" t="s">
+    <row r="163" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B163" s="1"/>
+      <c r="C163" s="7" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>

<commit_message>
importazione dati, diari, inizio gestione email + libreria bootstrap per multiselect option
</commit_message>
<xml_diff>
--- a/progettazione/requisitiLPI.xlsx
+++ b/progettazione/requisitiLPI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LPI\progettazione\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LPI\progettazione\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="92">
   <si>
     <t>ID</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>Prevedere l'eliminazione definitiva dei dati eliminati e ripristino</t>
+  </si>
+  <si>
+    <t>aggiunto in seguito, no su QdC</t>
   </si>
 </sst>
 </file>
@@ -666,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F166" sqref="F166"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H157" sqref="H157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1704,7 +1707,9 @@
       <c r="B161" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C161" s="3"/>
+      <c r="C161" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="162" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B162" s="1" t="s">

</xml_diff>

<commit_message>
correzioni di alcune cose dei test + piccole aggiunte e documentazione
</commit_message>
<xml_diff>
--- a/progettazione/requisitiLPI.xlsx
+++ b/progettazione/requisitiLPI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="105">
   <si>
     <t>ID</t>
   </si>
@@ -179,9 +179,6 @@
     <t>REQ-013</t>
   </si>
   <si>
-    <t>Pagine delle email</t>
-  </si>
-  <si>
     <t>Avere la possibilità di inviare email</t>
   </si>
   <si>
@@ -209,9 +206,6 @@
     <t>prevedere modal per la creazione dei datori di lavoro solo per gli amministratori</t>
   </si>
   <si>
-    <t>Salvare il file in pdf sul server</t>
-  </si>
-  <si>
     <t>REQ-014</t>
   </si>
   <si>
@@ -336,6 +330,15 @@
   </si>
   <si>
     <t>Può cambiare la password in caso di dimenticanza</t>
+  </si>
+  <si>
+    <t>Pagina delle email</t>
+  </si>
+  <si>
+    <t>Controllare la formattazione dei dati, soprattutto del contratto dell'apprendista</t>
+  </si>
+  <si>
+    <t>Salvare il file csv sul server</t>
   </si>
 </sst>
 </file>
@@ -703,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E179"/>
+  <dimension ref="B1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C175" sqref="B2:C175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,7 +744,7 @@
     </row>
     <row r="5" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -817,7 +820,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -830,7 +833,7 @@
     </row>
     <row r="20" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" s="4">
         <v>1</v>
@@ -865,7 +868,7 @@
     <row r="25" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="6"/>
       <c r="C25" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -883,7 +886,7 @@
     <row r="28" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="6"/>
       <c r="C28" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -895,13 +898,13 @@
     <row r="30" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="6"/>
       <c r="C30" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="6"/>
       <c r="C31" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -931,7 +934,7 @@
     </row>
     <row r="36" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C36" s="4">
         <v>1</v>
@@ -960,19 +963,19 @@
     <row r="40" spans="2:3" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="6"/>
       <c r="C40" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="6"/>
       <c r="C41" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="6"/>
       <c r="C42" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -984,25 +987,25 @@
     <row r="44" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B44" s="6"/>
       <c r="C44" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B45" s="6"/>
       <c r="C45" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="6"/>
       <c r="C46" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B47" s="6"/>
       <c r="C47" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1019,7 +1022,7 @@
         <v>2</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1032,7 +1035,7 @@
     </row>
     <row r="52" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C52" s="4">
         <v>1</v>
@@ -1061,13 +1064,13 @@
     <row r="56" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B56" s="6"/>
       <c r="C56" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B57" s="6"/>
       <c r="C57" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1079,7 +1082,7 @@
     <row r="59" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B59" s="6"/>
       <c r="C59" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1109,7 +1112,7 @@
     </row>
     <row r="64" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B64" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C64" s="4">
         <v>1</v>
@@ -1132,19 +1135,19 @@
     <row r="67" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B67" s="1"/>
       <c r="C67" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B68" s="5"/>
       <c r="C68" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="69" spans="2:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B69" s="6"/>
       <c r="C69" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1161,7 +1164,7 @@
         <v>2</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1174,7 +1177,7 @@
     </row>
     <row r="74" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B74" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C74" s="4">
         <v>1</v>
@@ -1200,7 +1203,7 @@
     <row r="77" spans="2:5" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B77" s="5"/>
       <c r="C77" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1230,7 +1233,7 @@
     </row>
     <row r="82" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B82" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C82" s="4">
         <v>1</v>
@@ -1270,7 +1273,7 @@
         <v>2</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1283,7 +1286,7 @@
     </row>
     <row r="90" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B90" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C90" s="4">
         <v>1</v>
@@ -1306,37 +1309,37 @@
     <row r="93" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B93" s="1"/>
       <c r="C93" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="94" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B94" s="1"/>
       <c r="C94" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="95" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B95" s="1"/>
       <c r="C95" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="96" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B96" s="5"/>
       <c r="C96" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="97" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B97" s="5"/>
       <c r="C97" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="98" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B98" s="5"/>
       <c r="C98" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1359,7 +1362,7 @@
         <v>2</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="103" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1372,7 +1375,7 @@
     </row>
     <row r="104" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B104" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C104" s="4">
         <v>1</v>
@@ -1395,13 +1398,13 @@
     <row r="107" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B107" s="5"/>
       <c r="C107" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="108" spans="2:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B108" s="5"/>
       <c r="C108" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="109" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1419,19 +1422,19 @@
     <row r="111" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B111" s="5"/>
       <c r="C111" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="112" spans="2:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B112" s="5"/>
       <c r="C112" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="113" spans="2:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B113" s="5"/>
       <c r="C113" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="114" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1454,7 +1457,7 @@
         <v>2</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="118" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1467,7 +1470,7 @@
     </row>
     <row r="119" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B119" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C119" s="4">
         <v>1</v>
@@ -1490,25 +1493,25 @@
     <row r="122" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B122" s="1"/>
       <c r="C122" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="123" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B123" s="5"/>
       <c r="C123" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="124" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B124" s="5"/>
       <c r="C124" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="125" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B125" s="5"/>
       <c r="C125" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="126" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1544,7 +1547,7 @@
     </row>
     <row r="131" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B131" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C131" s="4">
         <v>1</v>
@@ -1609,13 +1612,13 @@
     <row r="141" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B141" s="1"/>
       <c r="C141" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="142" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B142" s="1"/>
       <c r="C142" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="143" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1632,7 +1635,7 @@
         <v>2</v>
       </c>
       <c r="C145" s="7" t="s">
-        <v>51</v>
+        <v>102</v>
       </c>
     </row>
     <row r="146" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1645,7 +1648,7 @@
     </row>
     <row r="147" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B147" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C147" s="4">
         <v>1</v>
@@ -1674,31 +1677,31 @@
     <row r="151" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B151" s="1"/>
       <c r="C151" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="152" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B152" s="1"/>
       <c r="C152" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="153" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B153" s="1"/>
       <c r="C153" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="154" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B154" s="1"/>
       <c r="C154" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="155" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B155" s="1"/>
       <c r="C155" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="156" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1721,7 +1724,7 @@
         <v>2</v>
       </c>
       <c r="C159" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="160" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1734,10 +1737,10 @@
     </row>
     <row r="161" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B161" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="162" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1745,7 +1748,7 @@
         <v>4</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="163" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1759,81 +1762,87 @@
     <row r="164" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B164" s="1"/>
       <c r="C164" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="165" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B165" s="1"/>
       <c r="C165" s="7" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
     </row>
     <row r="166" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B166" s="1"/>
       <c r="C166" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="167" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="168" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B168" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="167" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B167" s="1"/>
+      <c r="C167" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="168" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="169" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B169" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C169" s="7" t="s">
-        <v>63</v>
+        <v>0</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="170" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B170" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C170" s="3">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C170" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="171" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B171" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C171" s="4" t="s">
-        <v>73</v>
+        <v>3</v>
+      </c>
+      <c r="C171" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="172" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B172" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>79</v>
+        <v>64</v>
+      </c>
+      <c r="C172" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="173" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B173" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="174" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B174" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C173" s="2" t="s">
+      <c r="C174" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="174" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B174" s="1"/>
-      <c r="C174" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="175" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="175" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B175" s="1"/>
+      <c r="C175" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
     <row r="176" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="177" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="178" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="179" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="180" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>